<commit_message>
update experiment details template
</commit_message>
<xml_diff>
--- a/det/DETAILSTEMPLATE.xlsx
+++ b/det/DETAILSTEMPLATE.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10311"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/simonlam/Library/CloudStorage/OneDrive-UniversityofCambridge/Projects/DDRcs/det/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thomas03/Library/CloudStorage/OneDrive-CRUKCambridgeInstitute/ddrcs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73918DA6-1E13-844A-82AC-AD2C7EDAAD3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72796A28-A0E6-B94A-A047-EA96090356D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17700" yWindow="1660" windowWidth="33500" windowHeight="25860" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13560" yWindow="14960" windowWidth="33500" windowHeight="20500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="7" r:id="rId1"/>
@@ -210,7 +210,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="36">
   <si>
     <t>Library</t>
   </si>
@@ -221,9 +221,6 @@
     <t>Representation average</t>
   </si>
   <si>
-    <t>Experiment description (a few sentences)</t>
-  </si>
-  <si>
     <t>Replicate</t>
   </si>
   <si>
@@ -296,22 +293,31 @@
     <t>DOI</t>
   </si>
   <si>
-    <t>Citation</t>
-  </si>
-  <si>
     <t>Name</t>
   </si>
   <si>
-    <t>analysis_version</t>
-  </si>
-  <si>
-    <t>file_prefix</t>
-  </si>
-  <si>
     <t>drugz</t>
   </si>
   <si>
     <t>mageck</t>
+  </si>
+  <si>
+    <t>Contrast</t>
+  </si>
+  <si>
+    <t>Experiment description</t>
+  </si>
+  <si>
+    <t>Notes about the analysis, e.g. a sample was excluded</t>
+  </si>
+  <si>
+    <t>A few sentences on the purpose of the experiment, and anything unusual in its design (e.g. it's a flow screen)</t>
+  </si>
+  <si>
+    <t>Reference</t>
+  </si>
+  <si>
+    <t>Required for screen viewer</t>
   </si>
 </sst>
 </file>
@@ -414,7 +420,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -422,16 +428,50 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -447,10 +487,17 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -802,16 +849,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
+      <xdr:col>4</xdr:col>
       <xdr:colOff>596900</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>139700</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
+      <xdr:col>12</xdr:col>
       <xdr:colOff>317500</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>165100</xdr:rowOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -826,8 +873,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4584700" y="139700"/>
-          <a:ext cx="5105400" cy="2946400"/>
+          <a:off x="7480300" y="139700"/>
+          <a:ext cx="5105400" cy="2654300"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -877,6 +924,26 @@
             <a:rPr lang="en-GB" sz="1400" baseline="0"/>
             <a:t>, "endpoints" and "otherprior", with additional info suffixed on, e.g. "endpoints_unpaired". Different groups can have different settings in the analyses sheet.</a:t>
           </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-GB" sz="1400" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1400" baseline="0"/>
+            <a:t>Contrast: a friendly name for the comparison, used in place of auto generated treatment names when given.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-GB" sz="1400" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1400" baseline="0"/>
+            <a:t>Comparison hexcode: an 8-digit hexadecimal code to uniquely identify this comparison, used in a future update</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
           <a:endParaRPr lang="en-GB" sz="1400"/>
         </a:p>
       </xdr:txBody>
@@ -1027,8 +1094,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E0A63A21-9CD2-8D4F-871C-3B6CE038B02C}" name="samp_deets2" displayName="samp_deets2" ref="A1:L3" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
-  <autoFilter ref="A1:L3" xr:uid="{E0A63A21-9CD2-8D4F-871C-3B6CE038B02C}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E0A63A21-9CD2-8D4F-871C-3B6CE038B02C}" name="samp_deets2" displayName="samp_deets2" ref="A1:L11" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+  <autoFilter ref="A1:L11" xr:uid="{E0A63A21-9CD2-8D4F-871C-3B6CE038B02C}"/>
   <tableColumns count="12">
     <tableColumn id="1" xr3:uid="{4A7B1510-870A-E341-BD37-430A1066E449}" name="Replicate"/>
     <tableColumn id="2" xr3:uid="{8287588F-8FD3-A646-94D4-43B56F35F2DB}" name="Sample"/>
@@ -1048,9 +1115,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1088,9 +1155,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1123,26 +1190,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1175,26 +1225,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1383,80 +1416,87 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="34.6640625" customWidth="1"/>
-    <col min="2" max="2" width="100.6640625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="100.6640625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="20">
+    <row r="1" spans="1:3" ht="20">
       <c r="A1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="10"/>
+    </row>
+    <row r="2" spans="1:3" ht="20">
+      <c r="A2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="2"/>
-    </row>
-    <row r="2" spans="1:2" ht="20">
-      <c r="A2" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B2" s="2"/>
-    </row>
-    <row r="3" spans="1:2" ht="20">
+      <c r="B2" s="11"/>
+    </row>
+    <row r="3" spans="1:3" ht="20">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="2"/>
-    </row>
-    <row r="4" spans="1:2" ht="20">
+      <c r="B3" s="11"/>
+      <c r="C3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="20">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="2"/>
-    </row>
-    <row r="5" spans="1:2" ht="20">
+      <c r="B4" s="11"/>
+    </row>
+    <row r="5" spans="1:3" ht="20">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="2"/>
-    </row>
-    <row r="6" spans="1:2" ht="40">
+      <c r="B5" s="11"/>
+    </row>
+    <row r="6" spans="1:3" ht="20">
       <c r="A6" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6" s="2"/>
-    </row>
-    <row r="7" spans="1:2" ht="20">
+        <v>31</v>
+      </c>
+      <c r="B6" s="11"/>
+      <c r="C6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="20">
       <c r="A7" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="20">
+        <v>10</v>
+      </c>
+      <c r="B7" s="12"/>
+      <c r="C7" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="20">
       <c r="A8" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="20">
+        <v>26</v>
+      </c>
+      <c r="B8" s="12"/>
+    </row>
+    <row r="9" spans="1:3" ht="21" thickBot="1">
       <c r="A9" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" ht="20">
-      <c r="A10" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" ht="20">
-      <c r="A11" s="1" t="s">
-        <v>31</v>
-      </c>
+        <v>34</v>
+      </c>
+      <c r="B9" s="13"/>
     </row>
   </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Alphanumeric only" error="Alphanumeric only." sqref="B1" xr:uid="{50DA87F9-C9A8-AD4D-851D-DCA4B42EAA51}">
+      <formula1>ISNUMBER(SUMPRODUCT(SEARCH(MID(B1,ROW(INDIRECT("1:"&amp;LEN(B1))),1),"0123456789abcdefghijklmnopqrstuvwxyzABCDEFGHIJKLMNOPQRSTUVWXYZ")))</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
@@ -1465,10 +1505,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:L3"/>
+  <dimension ref="A1:L11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -1488,76 +1528,146 @@
   <sheetData>
     <row r="1" spans="1:12" ht="20">
       <c r="A1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="E1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H1" s="5" t="s">
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="I1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="J1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="K1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>11</v>
-      </c>
     </row>
     <row r="2" spans="1:12" ht="22" customHeight="1">
-      <c r="A2" s="11"/>
-      <c r="B2" s="11"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="10"/>
-      <c r="G2" s="10"/>
-      <c r="H2" s="10"/>
-      <c r="I2" s="10"/>
-      <c r="J2" s="10"/>
-      <c r="K2" s="10"/>
-      <c r="L2" s="10"/>
+      <c r="B2" s="9"/>
+      <c r="C2" s="2"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
+      <c r="H2" s="8"/>
+      <c r="I2" s="8"/>
     </row>
     <row r="3" spans="1:12" ht="19">
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="10"/>
-      <c r="G3" s="10"/>
-      <c r="H3" s="10"/>
-      <c r="I3" s="10"/>
-      <c r="J3" s="10"/>
-      <c r="K3" s="10"/>
-      <c r="L3" s="10"/>
+      <c r="B3" s="9"/>
+      <c r="C3" s="2"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="8"/>
+      <c r="H3" s="8"/>
+      <c r="I3" s="8"/>
+    </row>
+    <row r="4" spans="1:12" ht="19">
+      <c r="B4" s="9"/>
+      <c r="C4" s="2"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="8"/>
+      <c r="G4" s="8"/>
+      <c r="H4" s="8"/>
+      <c r="I4" s="8"/>
+    </row>
+    <row r="5" spans="1:12" ht="19">
+      <c r="B5" s="9"/>
+      <c r="C5" s="2"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="8"/>
+      <c r="H5" s="8"/>
+      <c r="I5" s="8"/>
+    </row>
+    <row r="6" spans="1:12" ht="19">
+      <c r="B6" s="9"/>
+      <c r="C6" s="2"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="8"/>
+      <c r="H6" s="8"/>
+      <c r="I6" s="8"/>
+    </row>
+    <row r="7" spans="1:12" ht="19">
+      <c r="B7" s="9"/>
+      <c r="C7" s="2"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="8"/>
+      <c r="H7" s="8"/>
+      <c r="I7" s="8"/>
+    </row>
+    <row r="8" spans="1:12" ht="19">
+      <c r="B8" s="9"/>
+      <c r="C8" s="2"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="8"/>
+      <c r="G8" s="8"/>
+      <c r="H8" s="8"/>
+      <c r="I8" s="8"/>
+    </row>
+    <row r="9" spans="1:12" ht="19">
+      <c r="B9" s="9"/>
+      <c r="C9" s="2"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="8"/>
+      <c r="H9" s="8"/>
+      <c r="I9" s="8"/>
+    </row>
+    <row r="10" spans="1:12" ht="19">
+      <c r="B10" s="9"/>
+      <c r="C10" s="2"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="8"/>
+      <c r="H10" s="8"/>
+      <c r="I10" s="8"/>
+    </row>
+    <row r="11" spans="1:12" ht="19">
+      <c r="B11" s="9"/>
+      <c r="C11" s="2"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="8"/>
+      <c r="G11" s="8"/>
+      <c r="H11" s="8"/>
+      <c r="I11" s="8"/>
     </row>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
-  <dataValidations count="2">
+  <dataValidations count="4">
     <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Alphanumeric and fullstop, dash and underscore allowed." sqref="A1:A1048576" xr:uid="{63798D91-C498-4E49-B344-04A1C50A54F8}">
       <formula1>ISNUMBER(SUMPRODUCT(SEARCH(MID(A1,ROW(INDIRECT("1:"&amp;LEN(A1))),1),"0123456789abcdefghijklmnopqrstuvwxyzABCDEFGHIJKLMNOPQRSTUVWXYZ.-_–")))</formula1>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Disallowed character" error="Alphanumeric and underscores only allowed for sample name" sqref="B1:B1048576" xr:uid="{623F49ED-56E7-324A-A60D-33D3DBC40B4A}">
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Disallowed character" error="Alphanumeric and underscores only allowed for sample name" sqref="B1 B12:B1048576" xr:uid="{623F49ED-56E7-324A-A60D-33D3DBC40B4A}">
       <formula1>ISNUMBER(SUMPRODUCT(SEARCH(MID(B1,ROW(INDIRECT("1:"&amp;LEN(B1))),1),".+0123456789abcdefghijklmnopqrstuvwxyzABCDEFGHIJKLMNOPQRSTUVWXYZ_")))</formula1>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Disallowed character" error="Alphanumeric and underscores only allowed for sample name" sqref="B3:B11" xr:uid="{A7F92040-47E2-A048-B6EE-12FA19A04501}">
+      <formula1>ISNUMBER(SUMPRODUCT(SEARCH(MID(B3,ROW(INDIRECT("1:"&amp;LEN(B3))),1),"0123456789abcdefghijklmnopqrstuvwxyzABCDEFGHIJKLMNOPQRSTUVWXYZ_+")))</formula1>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Disallowed character" error="Alphanumeric and underscores only allowed for sample name. _x000a__x000a_Sample information gets encoded into output file names so other characters can cause issues. Periods and dashes will definitely cause issues." sqref="B2" xr:uid="{3311409A-3C35-594C-8482-10D739053B8B}">
+      <formula1>ISNUMBER(SUMPRODUCT(SEARCH(MID(B2,ROW(INDIRECT("1:"&amp;LEN(B2))),1),"0123456789abcdefghijklmnopqrstuvwxyzABCDEFGHIJKLMNOPQRSTUVWXYZ_+")))</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1570,51 +1680,39 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5852547F-8F24-4C5C-A576-33824D0B5E92}">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I23" sqref="I23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="16.5" customWidth="1"/>
     <col min="2" max="2" width="16.83203125" customWidth="1"/>
-    <col min="3" max="3" width="19" customWidth="1"/>
+    <col min="3" max="4" width="19" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="20">
+    <row r="1" spans="1:6" ht="20">
       <c r="A1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E1" s="7"/>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="B3" s="6"/>
-      <c r="C3" s="6"/>
-      <c r="E3" s="6"/>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="E4" s="6"/>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="E5" s="6"/>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="E6" s="6"/>
-    </row>
-    <row r="10" spans="1:5">
-      <c r="E10" s="6"/>
+      <c r="D1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F1" s="6"/>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="F2" s="5"/>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="F6" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1626,7 +1724,7 @@
           <x14:formula1>
             <xm:f>gubbins!$A:$A</xm:f>
           </x14:formula1>
-          <xm:sqref>B2:C102</xm:sqref>
+          <xm:sqref>B2:C98</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1638,9 +1736,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{779F645E-0A47-4C79-A34D-EC582264D863}">
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.5" defaultRowHeight="15"/>
   <cols>
@@ -1651,35 +1747,35 @@
   <sheetData>
     <row r="1" spans="1:7" ht="40">
       <c r="A1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>24</v>
-      </c>
       <c r="G1" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:7">
       <c r="C2" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="C3" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>